<commit_message>
Added the fixed groups size test pic
</commit_message>
<xml_diff>
--- a/experiments/Excel Charts/eps1.0,bud1.0,peers30,groups1-30,reg2e2-pubParty-groupsizetest-includelocal-adultmeanGroupSizeTest.xlsx
+++ b/experiments/Excel Charts/eps1.0,bud1.0,peers30,groups1-30,reg2e2-pubParty-groupsizetest-includelocal-adultmeanGroupSizeTest.xlsx
@@ -581,7 +581,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Error Rate</c:v>
+            <c:v>Group-publish</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -608,6 +608,95 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$A$1:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.17353771892299999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.168082377916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17052076646100001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17162961203499999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16957312568399999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16791764861299999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16671068230300001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>All-publish</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="rnd">
+                <a:noFill/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -615,60 +704,60 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$1:$C$7</c:f>
+                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$9:$C$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.7710944553999999E-3</c:v>
+                    <c:v>8.9405722650600001E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.1010917123700001E-3</c:v>
+                    <c:v>1.2920264879199999E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.4062641457099997E-3</c:v>
+                    <c:v>1.1887426402300001E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.7155099764899996E-3</c:v>
+                    <c:v>8.0737112486600001E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.1866512596700004E-3</c:v>
+                    <c:v>5.0199332734899996E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.11590084166E-3</c:v>
+                    <c:v>7.2856710083800001E-4</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.0431218218999997E-3</c:v>
+                    <c:v>5.5829984276799997E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$1:$C$7</c:f>
+                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$9:$C$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4.7710944553999999E-3</c:v>
+                    <c:v>8.9405722650600001E-4</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6.1010917123700001E-3</c:v>
+                    <c:v>1.2920264879199999E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>6.4062641457099997E-3</c:v>
+                    <c:v>1.1887426402300001E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.7155099764899996E-3</c:v>
+                    <c:v>8.0737112486600001E-4</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.1866512596700004E-3</c:v>
+                    <c:v>5.0199332734899996E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>5.11590084166E-3</c:v>
+                    <c:v>7.2856710083800001E-4</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.0431218218999997E-3</c:v>
+                    <c:v>5.5829984276799997E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -689,7 +778,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$A$1:$A$7</c:f>
+              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$A$9:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -719,30 +808,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$B$1:$B$7</c:f>
+              <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$B$9:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.17353771892299999</c:v>
+                  <c:v>0.16573633888200001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.168082377916</c:v>
+                  <c:v>0.16465000102399999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17052076646100001</c:v>
+                  <c:v>0.16541612922999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17162961203499999</c:v>
+                  <c:v>0.164807034785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16957312568399999</c:v>
+                  <c:v>0.16485780971700001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16791764861299999</c:v>
+                  <c:v>0.16481358638900001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16671068230300001</c:v>
+                  <c:v>0.16453022951099999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,11 +846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280530304"/>
-        <c:axId val="280528624"/>
+        <c:axId val="185100256"/>
+        <c:axId val="185100816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280530304"/>
+        <c:axId val="185100256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,16 +963,16 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280528624"/>
+        <c:crossAx val="185100816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280528624"/>
+        <c:axId val="185100816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.70000000000000007"/>
-          <c:min val="0"/>
+          <c:max val="0.2"/>
+          <c:min val="0.15000000000000002"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -994,7 +1083,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280530304"/>
+        <c:crossAx val="185100256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1990,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="C9" sqref="C9:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,6 +2164,83 @@
         <v>4.0431218218999997E-3</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0.16573633888200001</v>
+      </c>
+      <c r="C9">
+        <v>8.9405722650600001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.16465000102399999</v>
+      </c>
+      <c r="C10">
+        <v>1.2920264879199999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.16541612922999999</v>
+      </c>
+      <c r="C11">
+        <v>1.1887426402300001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.164807034785</v>
+      </c>
+      <c r="C12">
+        <v>8.0737112486600001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>0.16485780971700001</v>
+      </c>
+      <c r="C13">
+        <v>5.0199332734899996E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>0.16481358638900001</v>
+      </c>
+      <c r="C14">
+        <v>7.2856710083800001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>0.16453022951099999</v>
+      </c>
+      <c r="C15">
+        <v>5.5829984276799997E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated gpst excel chart
</commit_message>
<xml_diff>
--- a/experiments/Excel Charts/eps1.0,bud1.0,peers30,groups1-30,reg2e2-pubParty-groupsizetest-includelocal-adultmeanGroupSizeTest.xlsx
+++ b/experiments/Excel Charts/eps1.0,bud1.0,peers30,groups1-30,reg2e2-pubParty-groupsizetest-includelocal-adultmeanGroupSizeTest.xlsx
@@ -592,7 +592,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:pattFill prst="solidDmnd">
                 <a:fgClr>
@@ -608,6 +608,83 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$1:$C$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.7710944553999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.1010917123700001E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.4062641457099997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.7155099764899996E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.1866512596700004E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.11590084166E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0431218218999997E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$C$1:$C$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.7710944553999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.1010917123700001E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>6.4062641457099997E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.7155099764899996E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.1866512596700004E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.11590084166E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0431218218999997E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+                <a:tailEnd type="diamond"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'eps1.0,bud1.0,peers30,groups1-3'!$A$1:$A$7</c:f>
@@ -685,21 +762,24 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="diamond"/>
-            <c:size val="10"/>
+            <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525" cap="rnd">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
                 <a:miter lim="800000"/>
+                <a:tailEnd type="arrow" w="sm" len="med"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
-            <c:errBarType val="both"/>
+            <c:errBarType val="plus"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
@@ -766,12 +846,10 @@
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:round/>
+                <a:tailEnd type="oval" w="sm" len="sm"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -846,11 +924,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185100256"/>
-        <c:axId val="185100816"/>
+        <c:axId val="185341232"/>
+        <c:axId val="185341792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185100256"/>
+        <c:axId val="185341232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,16 +1041,16 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185100816"/>
+        <c:crossAx val="185341792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185100816"/>
+        <c:axId val="185341792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.2"/>
-          <c:min val="0.15000000000000002"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1083,7 +1161,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185100256"/>
+        <c:crossAx val="185341232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>